<commit_message>
added date tests to convert sql dates to string
</commit_message>
<xml_diff>
--- a/merlinserver/src/test/resources/datesdata.xlsx
+++ b/merlinserver/src/test/resources/datesdata.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="10335" xr2:uid="{1472B959-D15D-433A-ADCF-FF0A66E4797D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12585" windowHeight="10335" xr2:uid="{1472B959-D15D-433A-ADCF-FF0A66E4797D}"/>
   </bookViews>
   <sheets>
-    <sheet name="dates" sheetId="1" r:id="rId1"/>
-    <sheet name="lists" sheetId="2" r:id="rId2"/>
+    <sheet name="dates" sheetId="3" r:id="rId1"/>
+    <sheet name="datestrings" sheetId="1" r:id="rId2"/>
+    <sheet name="lists" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:H32"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Format</t>
   </si>
@@ -54,6 +55,30 @@
   </si>
   <si>
     <t>11//21//2000</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/11/2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11 Nov 2000</t>
+  </si>
+  <si>
+    <t>abndna</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/11/2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-11-2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Nov 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-11-2000</t>
   </si>
 </sst>
 </file>
@@ -89,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,17 +431,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B78264F-9937-4D89-B36F-6016C55AE8A2}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C084A061-7EDD-4C60-82E2-05FC21367DB1}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -432,66 +458,87 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>36851</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>36851</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>36851</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>36841</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="B6" s="2">
+        <v>36841</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>36841</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56B9FAE0-7541-4126-9D2B-E9F2EA9BF022}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F4C3B05-5D49-4941-B8AD-BC90B754075A}">
           <x14:formula1>
-            <xm:f>lists!$A$2:$A$3</xm:f>
+            <xm:f>lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{094EE1F3-E5FB-4CF2-99AE-A4826BE48336}">
-          <x14:formula1>
-            <xm:f>lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C5</xm:sqref>
+          <xm:sqref>A2:A7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -500,11 +547,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F409B5E3-F86B-4629-BC4D-FACC56E99895}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B78264F-9937-4D89-B36F-6016C55AE8A2}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>36851</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>36841</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{094EE1F3-E5FB-4CF2-99AE-A4826BE48336}">
+          <x14:formula1>
+            <xm:f>lists!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F409B5E3-F86B-4629-BC4D-FACC56E99895}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +681,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated dateutil, -removed front controller -removed web.xml -updated ng tests
</commit_message>
<xml_diff>
--- a/merlinserver/src/test/resources/datesdata.xlsx
+++ b/merlinserver/src/test/resources/datesdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luie\Desktop\work\revature\project2\Server\Merlin\merlinserver\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12585" windowHeight="10335" xr2:uid="{1472B959-D15D-433A-ADCF-FF0A66E4797D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="9105" xr2:uid="{1472B959-D15D-433A-ADCF-FF0A66E4797D}"/>
   </bookViews>
   <sheets>
     <sheet name="dates" sheetId="3" r:id="rId1"/>
@@ -12,7 +17,6 @@
     <sheet name="lists" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H32"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>Format</t>
   </si>
@@ -36,15 +40,6 @@
     <t>20/11/2001</t>
   </si>
   <si>
-    <t>dash</t>
-  </si>
-  <si>
-    <t>slash</t>
-  </si>
-  <si>
-    <t>Formats</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -57,12 +52,6 @@
     <t>11//21//2000</t>
   </si>
   <si>
-    <t>space</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11/11/2000</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 11 Nov 2000</t>
   </si>
   <si>
@@ -78,7 +67,232 @@
     <t xml:space="preserve"> 21 Nov 2000</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11-11-2000</t>
+    <t>dd-MM-yyyy</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>dd-MMM-yyyy</t>
+  </si>
+  <si>
+    <t>dd MMMM yyyy</t>
+  </si>
+  <si>
+    <t>dd-MM-yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy  hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd-MMM-yyyy  hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd MMMM yyyy  hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd-MM-yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy  hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd-MMM-yyyy  hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd MMMM yyyy  hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd MMM yyyy</t>
+  </si>
+  <si>
+    <t>dd MMM yyyy  hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd MMM yyyy  hh:mm:ss a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-Nov-2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 November 2000</t>
+  </si>
+  <si>
+    <t>11 21 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-21-2000</t>
+  </si>
+  <si>
+    <t>November 21 2000</t>
+  </si>
+  <si>
+    <t>Nov 21 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November 21, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/11/2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-11-2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Nov 2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-Nov-2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 November 2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/11/2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-11-2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Nov 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-Nov-2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 November 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/11/2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-11-2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Nov 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21-Nov-2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 November 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-21-2000 01:11:11</t>
+  </si>
+  <si>
+    <t>Nov 21 2000 01:11:11</t>
+  </si>
+  <si>
+    <t>November 21 2000 01:11:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November 21, 2000 01:11:11</t>
+  </si>
+  <si>
+    <t>11 21 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-21-2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t>Nov 21 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t>November 21 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November 21, 2000 01:11:11 AM</t>
+  </si>
+  <si>
+    <t>11 21 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11-21-2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t>Nov 21 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t>November 21 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November 21, 2000 01:11:11 PM</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy</t>
+  </si>
+  <si>
+    <t>Date ForMats</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>MM dd yyyy</t>
+  </si>
+  <si>
+    <t>MMM dd yyyy</t>
+  </si>
+  <si>
+    <t>MMMM dd yyyy</t>
+  </si>
+  <si>
+    <t>MMMM dd, yyyy</t>
+  </si>
+  <si>
+    <t>MM dd yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>MMM dd yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>MMMM dd yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>MMMM dd, yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>MM dd yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>MMM dd yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>MMMM dd yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>MMMM dd, yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd MMM yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd-MMM-yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd MMMM yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd MMM yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd-MMM-yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>dd MMMM yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>11 21 2000 01:11:11</t>
   </si>
 </sst>
 </file>
@@ -114,10 +328,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,17 +648,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C084A061-7EDD-4C60-82E2-05FC21367DB1}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,81 +668,450 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>36851</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>36851</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>36851</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36851</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>36851</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>36841</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>36841</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>36841</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B8" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="4">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="4">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="4">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="4">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="1">
+        <v>36851.049432870372</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1">
+        <v>36851.549432870372</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -536,9 +1121,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F4C3B05-5D49-4941-B8AD-BC90B754075A}">
           <x14:formula1>
-            <xm:f>lists!$A$2:$A$4</xm:f>
+            <xm:f>lists!$A$2:$A$31</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A7</xm:sqref>
+          <xm:sqref>A2:A41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -548,7 +1133,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B78264F-9937-4D89-B36F-6016C55AE8A2}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -560,74 +1145,70 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36851</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>36841</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,41 +1230,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F409B5E3-F86B-4629-BC4D-FACC56E99895}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>